<commit_message>
Normalize shipping data and add finance dataset
Standardize shipping records: replace verbose delivery messages with structured fields (fee, status, date), update _id and customer_id values across data/shipping.json, and adjust related assets (shipping_data.xlsx). Add new data/finance.json with sample monthly deposits. Update .claude/settings.local.json to include a PYTHONIOENCODING Bash wrapper. Modify scripts and assets (db_refresh.py, export_mongo.py, js/app.js, img/icon.png) and add/remove icons (add img/icon_0.png, remove img/icon_1.png) to reflect the data/schema changes.
</commit_message>
<xml_diff>
--- a/data/shipping_data.xlsx
+++ b/data/shipping_data.xlsx
@@ -5,22 +5,35 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Project Files\Daily Python\Day11\flaskProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\DesktopFiles\Cupstock\shuangshuangstore\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EADDE33-2E8D-4FCC-8A1A-3C2702C3C346}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{937F5B31-45FB-457E-B4BC-EE44A1E1942E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2860" yWindow="580" windowWidth="32410" windowHeight="19700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1770" yWindow="840" windowWidth="33730" windowHeight="19700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="218">
   <si>
     <t>tracking_number</t>
   </si>
@@ -668,6 +681,12 @@
   </si>
   <si>
     <t>1*30oz粉包装 +4*40oz蓝包装+2*情人节款30oz包装+1*情人节款红色30oz包装</t>
+  </si>
+  <si>
+    <t>fee</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
@@ -794,7 +813,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -827,6 +846,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1131,10 +1151,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H64"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43:D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.4"/>
@@ -1142,14 +1162,16 @@
     <col min="1" max="1" width="19.08984375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.1796875" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.90625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="143.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.1796875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="75.7265625" style="4" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="49.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="143.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.1796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="17.1796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="75.7265625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="49.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1160,22 +1182,28 @@
         <v>2</v>
       </c>
       <c r="D1" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="E1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="F1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="G1" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="H1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="I1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1185,21 +1213,28 @@
       <c r="C2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="4">
+      <c r="G2" s="4">
+        <f>F2*4</f>
+        <v>40</v>
+      </c>
+      <c r="H2" s="4">
         <v>17757227637</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H2" s="8"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="J2" s="8"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -1209,21 +1244,28 @@
       <c r="C3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4">
+        <f t="shared" ref="G3:G64" si="0">F3*4</f>
+        <v>34</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="8"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="J3" s="8"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -1233,23 +1275,30 @@
       <c r="C4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F4" s="4">
+      <c r="G4" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H4" s="4">
         <v>18620218340</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="8" t="s">
+      <c r="J4" s="8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -1259,23 +1308,30 @@
       <c r="C5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F5" s="4">
+      <c r="G5" s="4">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H5" s="4">
         <v>18221208628</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="J5" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -1285,23 +1341,30 @@
       <c r="C6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="G6" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="I6" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="J6" s="8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="10" t="s">
         <v>13</v>
       </c>
@@ -1311,21 +1374,28 @@
       <c r="C7" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="F7" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="11">
+      <c r="G7" s="4">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="H7" s="11">
         <v>18268360779</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="I7" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="H7" s="12"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="J7" s="12"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -1335,21 +1405,28 @@
       <c r="C8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="4">
+      <c r="G8" s="4">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="H8" s="4">
         <v>17336298533</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="I8" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="H8" s="8"/>
-    </row>
-    <row r="9" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="J8" s="8"/>
+    </row>
+    <row r="9" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="10" t="s">
         <v>15</v>
       </c>
@@ -1359,21 +1436,28 @@
       <c r="C9" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="F9" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="11">
+      <c r="G9" s="4">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="H9" s="11">
         <v>13967256688</v>
       </c>
-      <c r="G9" s="11" t="s">
+      <c r="I9" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="H9" s="12"/>
-    </row>
-    <row r="10" spans="1:8" s="13" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="J9" s="12"/>
+    </row>
+    <row r="10" spans="1:10" s="13" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A10" s="10" t="s">
         <v>16</v>
       </c>
@@ -1383,21 +1467,28 @@
       <c r="C10" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="F10" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="11">
+      <c r="G10" s="4">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="H10" s="11">
         <v>17757227637</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="I10" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="H10" s="12"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="J10" s="12"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
@@ -1407,23 +1498,30 @@
       <c r="C11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E11" s="4">
+      <c r="F11" s="4">
         <v>2.5</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="G11" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="I11" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="J11" s="8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
@@ -1433,23 +1531,30 @@
       <c r="C12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E12" s="4">
+      <c r="F12" s="4">
         <v>2.5</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="G12" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H12" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="4" t="s">
+      <c r="I12" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="H12" s="8" t="s">
+      <c r="J12" s="8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
         <v>19</v>
       </c>
@@ -1459,23 +1564,30 @@
       <c r="C13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="4">
+      <c r="F13" s="4">
         <v>8</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="G13" s="4">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="I13" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="J13" s="8" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
         <v>59</v>
       </c>
@@ -1485,21 +1597,28 @@
       <c r="C14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E14" s="4">
+      <c r="F14" s="4">
         <v>10.5</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="G14" s="4">
+        <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="H14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I14" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="H14" s="8"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="J14" s="8"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
         <v>60</v>
       </c>
@@ -1509,21 +1628,28 @@
       <c r="C15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="4">
+      <c r="F15" s="4">
         <v>10</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="G15" s="4">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="H15" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G15" s="5" t="s">
+      <c r="I15" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="H15" s="8"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="J15" s="8"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
         <v>66</v>
       </c>
@@ -1533,21 +1659,28 @@
       <c r="C16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E16" s="4">
+      <c r="F16" s="4">
         <v>3</v>
       </c>
-      <c r="F16" s="4">
+      <c r="G16" s="4">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H16" s="4">
         <v>13705017817</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="I16" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="H16" s="8"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="J16" s="8"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
         <v>70</v>
       </c>
@@ -1557,21 +1690,28 @@
       <c r="C17" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E17" s="4">
+      <c r="F17" s="4">
         <v>8.5</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="G17" s="4">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="H17" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="I17" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="H17" s="8"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="J17" s="8"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
         <v>73</v>
       </c>
@@ -1581,21 +1721,28 @@
       <c r="C18" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="E18" s="4">
+      <c r="F18" s="4">
         <v>9</v>
       </c>
-      <c r="F18" s="4" t="s">
+      <c r="G18" s="4">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="H18" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="I18" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="H18" s="8"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="J18" s="8"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A19" s="3" t="s">
         <v>75</v>
       </c>
@@ -1605,21 +1752,28 @@
       <c r="C19" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E19" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E19" s="4">
+      <c r="F19" s="4">
         <v>8.5</v>
       </c>
-      <c r="F19" s="4">
+      <c r="G19" s="4">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="H19" s="4">
         <v>17757227637</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="I19" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="H19" s="8"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="J19" s="8"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A20" s="3" t="s">
         <v>76</v>
       </c>
@@ -1629,21 +1783,28 @@
       <c r="C20" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E20" s="4">
+      <c r="F20" s="4">
         <v>8.5</v>
       </c>
-      <c r="F20" s="4" t="s">
+      <c r="G20" s="4">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="H20" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="I20" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="H20" s="8"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="J20" s="8"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
         <v>79</v>
       </c>
@@ -1653,21 +1814,28 @@
       <c r="C21" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E21" s="4">
+      <c r="F21" s="4">
         <v>8.5</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="G21" s="4">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="H21" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="I21" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="H21" s="8"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
         <v>81</v>
       </c>
@@ -1677,21 +1845,28 @@
       <c r="C22" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E22" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="E22" s="4">
+      <c r="F22" s="4">
         <v>9</v>
       </c>
-      <c r="F22" s="4" t="s">
+      <c r="G22" s="4">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="H22" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="I22" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="H22" s="8"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="J22" s="8"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
         <v>83</v>
       </c>
@@ -1701,21 +1876,28 @@
       <c r="C23" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E23" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E23" s="4">
+      <c r="F23" s="4">
         <v>9</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="G23" s="4">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="H23" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="I23" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="H23" s="8"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="J23" s="8"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
         <v>84</v>
       </c>
@@ -1725,21 +1907,28 @@
       <c r="C24" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E24" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="E24" s="4">
+      <c r="F24" s="4">
         <v>9</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="G24" s="4">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="H24" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="I24" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="H24" s="8"/>
-    </row>
-    <row r="25" spans="1:8" s="8" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="J24" s="8"/>
+    </row>
+    <row r="25" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A25" s="3" t="s">
         <v>101</v>
       </c>
@@ -1749,20 +1938,27 @@
       <c r="C25" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E25" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E25" s="4">
+      <c r="F25" s="4">
         <v>8.5</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="G25" s="4">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="H25" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="I25" s="5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A26" s="3" t="s">
         <v>95</v>
       </c>
@@ -1772,21 +1968,28 @@
       <c r="C26" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E26" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="E26" s="4">
+      <c r="F26" s="4">
         <v>7.5</v>
       </c>
-      <c r="F26" s="4">
+      <c r="G26" s="4">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="H26" s="4">
         <v>13616296429</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="I26" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="H26" s="8"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="J26" s="8"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A27" s="2" t="s">
         <v>97</v>
       </c>
@@ -1796,21 +1999,28 @@
       <c r="C27" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E27" s="4">
+      <c r="F27" s="4">
         <v>7.5</v>
       </c>
-      <c r="F27" s="4">
+      <c r="G27" s="4">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="H27" s="4">
         <v>13615826555</v>
       </c>
-      <c r="G27" s="3" t="s">
+      <c r="I27" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="H27" s="8"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="J27" s="8"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A28" s="3" t="s">
         <v>86</v>
       </c>
@@ -1820,21 +2030,28 @@
       <c r="C28" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E28" s="4">
+      <c r="F28" s="4">
         <v>2</v>
       </c>
-      <c r="F28" s="4">
+      <c r="G28" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H28" s="4">
         <v>13061289812</v>
       </c>
-      <c r="G28" s="4" t="s">
+      <c r="I28" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="H28" s="8"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="J28" s="8"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A29" s="3" t="s">
         <v>93</v>
       </c>
@@ -1844,21 +2061,28 @@
       <c r="C29" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E29" s="4">
+      <c r="F29" s="4">
         <v>2</v>
       </c>
-      <c r="F29" s="4">
+      <c r="G29" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H29" s="4">
         <v>13164556692</v>
       </c>
-      <c r="G29" s="4" t="s">
+      <c r="I29" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="H29" s="8"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="J29" s="8"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A30" s="9" t="s">
         <v>105</v>
       </c>
@@ -1868,20 +2092,27 @@
       <c r="C30" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E30" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="E30" s="4">
+      <c r="F30" s="4">
         <v>9.5</v>
       </c>
-      <c r="F30" s="4">
+      <c r="G30" s="4">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="H30" s="4">
         <v>13967256688</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="I30" s="5" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A31" s="2" t="s">
         <v>107</v>
       </c>
@@ -1891,20 +2122,27 @@
       <c r="C31" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E31" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="E31" s="4">
+      <c r="F31" s="4">
         <v>9.5</v>
       </c>
-      <c r="F31" s="4">
+      <c r="G31" s="4">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="H31" s="4">
         <v>15967207558</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="I31" s="5" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A32" s="3" t="s">
         <v>110</v>
       </c>
@@ -1914,20 +2152,27 @@
       <c r="C32" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E32" s="4">
+      <c r="F32" s="4">
         <v>2.5</v>
       </c>
-      <c r="F32" s="4">
+      <c r="G32" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H32" s="4">
         <v>13389943159</v>
       </c>
-      <c r="G32" s="4" t="s">
+      <c r="I32" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A33" s="3" t="s">
         <v>116</v>
       </c>
@@ -1937,20 +2182,27 @@
       <c r="C33" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E33" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="E33" s="4">
+      <c r="F33" s="4">
         <v>3</v>
       </c>
-      <c r="F33" s="4">
+      <c r="G33" s="4">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H33" s="4">
         <v>13750073375</v>
       </c>
-      <c r="G33" s="4" t="s">
+      <c r="I33" s="4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A34" s="2" t="s">
         <v>125</v>
       </c>
@@ -1960,20 +2212,27 @@
       <c r="C34" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="E34" s="4">
+      <c r="F34" s="4">
         <v>3</v>
       </c>
-      <c r="F34" s="4">
+      <c r="G34" s="4">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H34" s="4">
         <v>13510185811</v>
       </c>
-      <c r="G34" s="4" t="s">
+      <c r="I34" s="4" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A35" s="2" t="s">
         <v>123</v>
       </c>
@@ -1983,20 +2242,27 @@
       <c r="C35" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E35" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="E35" s="4">
+      <c r="F35" s="4">
         <v>5</v>
       </c>
-      <c r="F35" s="4">
+      <c r="G35" s="4">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="H35" s="4">
         <v>18880831409</v>
       </c>
-      <c r="G35" s="4" t="s">
+      <c r="I35" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A36" s="3" t="s">
         <v>127</v>
       </c>
@@ -2006,20 +2272,27 @@
       <c r="C36" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E36" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E36" s="4">
+      <c r="F36" s="4">
         <v>2.5</v>
       </c>
-      <c r="F36" s="4">
+      <c r="G36" s="4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="H36" s="4">
         <v>15976941831</v>
       </c>
-      <c r="G36" s="4" t="s">
+      <c r="I36" s="4" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A37" s="3" t="s">
         <v>131</v>
       </c>
@@ -2029,20 +2302,27 @@
       <c r="C37" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="E37" s="4">
+      <c r="F37" s="4">
         <v>9</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="G37" s="4">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="H37" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G37" s="4" t="s">
+      <c r="I37" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A38" s="3" t="s">
         <v>132</v>
       </c>
@@ -2052,20 +2332,27 @@
       <c r="C38" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="E38" s="4">
+      <c r="F38" s="4">
         <v>8.5</v>
       </c>
-      <c r="F38" s="4">
+      <c r="G38" s="4">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="H38" s="4">
         <v>15757278066</v>
       </c>
-      <c r="G38" s="4" t="s">
+      <c r="I38" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A39" s="3" t="s">
         <v>133</v>
       </c>
@@ -2075,20 +2362,27 @@
       <c r="C39" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E39" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="E39" s="4">
+      <c r="F39" s="4">
         <v>8</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="G39" s="4">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="H39" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G39" s="2" t="s">
+      <c r="I39" s="2" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="40" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A40" s="2" t="s">
         <v>143</v>
       </c>
@@ -2098,23 +2392,30 @@
       <c r="C40" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E40" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="E40" s="4">
+      <c r="F40" s="4">
         <v>3</v>
       </c>
-      <c r="F40" s="4">
+      <c r="G40" s="4">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H40" s="4">
         <v>13952090104</v>
       </c>
-      <c r="G40" s="2" t="s">
+      <c r="I40" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="H40" s="3" t="s">
+      <c r="J40" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="41" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A41" s="3" t="s">
         <v>144</v>
       </c>
@@ -2124,23 +2425,30 @@
       <c r="C41" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="D41" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E41" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="E41" s="4">
+      <c r="F41" s="4">
         <v>10.5</v>
       </c>
-      <c r="F41" s="4">
+      <c r="G41" s="4">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="H41" s="4">
         <v>13615826555</v>
       </c>
-      <c r="G41" s="4" t="s">
+      <c r="I41" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="H41" s="3" t="s">
+      <c r="J41" s="3" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A42" s="3" t="s">
         <v>149</v>
       </c>
@@ -2150,20 +2458,27 @@
       <c r="C42" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="16">
+        <v>46020</v>
+      </c>
+      <c r="E42" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="E42" s="4">
+      <c r="F42" s="4">
         <v>4</v>
       </c>
-      <c r="F42" s="4">
+      <c r="G42" s="4">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="H42" s="4">
         <v>15757278066</v>
       </c>
-      <c r="G42" s="4" t="s">
+      <c r="I42" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A43" s="3" t="s">
         <v>152</v>
       </c>
@@ -2173,20 +2488,27 @@
       <c r="C43" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D43" s="6" t="s">
+      <c r="D43" s="16">
+        <v>46048</v>
+      </c>
+      <c r="E43" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="E43" s="4">
+      <c r="F43" s="4">
         <v>9.5</v>
       </c>
-      <c r="F43" s="4" t="s">
+      <c r="G43" s="4">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="H43" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G43" s="2" t="s">
+      <c r="I43" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A44" s="3" t="s">
         <v>153</v>
       </c>
@@ -2196,20 +2518,27 @@
       <c r="C44" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D44" s="6" t="s">
+      <c r="D44" s="16">
+        <v>46048</v>
+      </c>
+      <c r="E44" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="E44" s="4">
+      <c r="F44" s="4">
         <v>9.5</v>
       </c>
-      <c r="F44" s="4">
+      <c r="G44" s="4">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="H44" s="4">
         <v>15757278066</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="I44" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A45" s="3" t="s">
         <v>154</v>
       </c>
@@ -2219,20 +2548,27 @@
       <c r="C45" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D45" s="6" t="s">
+      <c r="D45" s="16">
+        <v>46048</v>
+      </c>
+      <c r="E45" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="E45" s="4">
+      <c r="F45" s="4">
         <v>9</v>
       </c>
-      <c r="F45" s="4" t="s">
+      <c r="G45" s="4">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="H45" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G45" s="2" t="s">
+      <c r="I45" s="2" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A46" s="3" t="s">
         <v>155</v>
       </c>
@@ -2242,20 +2578,27 @@
       <c r="C46" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D46" s="6" t="s">
+      <c r="D46" s="16">
+        <v>46048</v>
+      </c>
+      <c r="E46" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="E46" s="4">
+      <c r="F46" s="4">
         <v>16</v>
       </c>
-      <c r="F46" s="4">
+      <c r="G46" s="4">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="H46" s="4">
         <v>13967256688</v>
       </c>
-      <c r="G46" s="2" t="s">
+      <c r="I46" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A47" s="3" t="s">
         <v>156</v>
       </c>
@@ -2265,20 +2608,27 @@
       <c r="C47" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D47" s="6" t="s">
+      <c r="D47" s="16">
+        <v>46048</v>
+      </c>
+      <c r="E47" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="E47" s="4">
+      <c r="F47" s="4">
         <v>11</v>
       </c>
-      <c r="F47" s="4">
+      <c r="G47" s="4">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="H47" s="4">
         <v>15967207558</v>
       </c>
-      <c r="G47" s="4" t="s">
+      <c r="I47" s="4" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A48" s="3" t="s">
         <v>164</v>
       </c>
@@ -2288,20 +2638,27 @@
       <c r="C48" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D48" s="3" t="s">
+      <c r="D48" s="16">
+        <v>46048</v>
+      </c>
+      <c r="E48" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E48" s="4">
+      <c r="F48" s="4">
         <v>2</v>
       </c>
-      <c r="F48" s="4">
+      <c r="G48" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H48" s="4">
         <v>18750197736</v>
       </c>
-      <c r="G48" s="4" t="s">
+      <c r="I48" s="4" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A49" s="3" t="s">
         <v>172</v>
       </c>
@@ -2311,20 +2668,27 @@
       <c r="C49" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" s="16">
+        <v>46048</v>
+      </c>
+      <c r="E49" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="E49" s="4">
+      <c r="F49" s="4">
         <v>3</v>
       </c>
-      <c r="F49" s="4">
+      <c r="G49" s="4">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H49" s="4">
         <v>19884385459</v>
       </c>
-      <c r="G49" s="4" t="s">
+      <c r="I49" s="4" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A50" s="3" t="s">
         <v>171</v>
       </c>
@@ -2334,20 +2698,27 @@
       <c r="C50" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="D50" s="16">
+        <v>46048</v>
+      </c>
+      <c r="E50" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="E50" s="4">
+      <c r="F50" s="4">
         <v>3</v>
       </c>
-      <c r="F50" s="4">
+      <c r="G50" s="4">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H50" s="4">
         <v>17367931585</v>
       </c>
-      <c r="G50" s="4" t="s">
+      <c r="I50" s="4" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A51" s="3" t="s">
         <v>178</v>
       </c>
@@ -2357,20 +2728,27 @@
       <c r="C51" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D51" s="3" t="s">
+      <c r="D51" s="16">
+        <v>46048</v>
+      </c>
+      <c r="E51" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E51" s="4">
+      <c r="F51" s="4">
         <v>2</v>
       </c>
-      <c r="F51" s="4">
+      <c r="G51" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H51" s="4">
         <v>13724149015</v>
       </c>
-      <c r="G51" s="4" t="s">
+      <c r="I51" s="4" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A52" s="3" t="s">
         <v>177</v>
       </c>
@@ -2380,20 +2758,27 @@
       <c r="C52" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" s="16">
+        <v>46048</v>
+      </c>
+      <c r="E52" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="E52" s="4">
+      <c r="F52" s="4">
         <v>3</v>
       </c>
-      <c r="F52" s="4">
+      <c r="G52" s="4">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="H52" s="4">
         <v>15882130778</v>
       </c>
-      <c r="G52" s="4" t="s">
+      <c r="I52" s="4" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A53" s="3" t="s">
         <v>185</v>
       </c>
@@ -2403,20 +2788,27 @@
       <c r="C53" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D53" s="3" t="s">
+      <c r="D53" s="16">
+        <v>46048</v>
+      </c>
+      <c r="E53" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="E53" s="4">
+      <c r="F53" s="4">
         <v>3.5</v>
       </c>
-      <c r="F53" s="4">
+      <c r="G53" s="4">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="H53" s="4">
         <v>18875030107</v>
       </c>
-      <c r="G53" s="4" t="s">
+      <c r="I53" s="4" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A54" s="3" t="s">
         <v>186</v>
       </c>
@@ -2426,20 +2818,27 @@
       <c r="C54" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="D54" s="16">
+        <v>46048</v>
+      </c>
+      <c r="E54" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="E54" s="4">
+      <c r="F54" s="4">
         <v>2</v>
       </c>
-      <c r="F54" s="4">
+      <c r="G54" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H54" s="4">
         <v>13965278525</v>
       </c>
-      <c r="G54" s="4" t="s">
+      <c r="I54" s="4" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A55" s="3" t="s">
         <v>189</v>
       </c>
@@ -2449,20 +2848,27 @@
       <c r="C55" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="D55" s="16">
+        <v>46048</v>
+      </c>
+      <c r="E55" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E55" s="4">
+      <c r="F55" s="4">
         <v>2</v>
       </c>
-      <c r="F55" s="4">
+      <c r="G55" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H55" s="4">
         <v>15253177715</v>
       </c>
-      <c r="G55" s="4" t="s">
+      <c r="I55" s="4" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A56" s="3" t="s">
         <v>191</v>
       </c>
@@ -2472,20 +2878,27 @@
       <c r="C56" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="D56" s="16">
+        <v>46048</v>
+      </c>
+      <c r="E56" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E56" s="4">
+      <c r="F56" s="4">
         <v>2</v>
       </c>
-      <c r="F56" s="4">
+      <c r="G56" s="4">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H56" s="4">
         <v>15342205101</v>
       </c>
-      <c r="G56" s="4" t="s">
+      <c r="I56" s="4" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A57" s="3" t="s">
         <v>194</v>
       </c>
@@ -2495,20 +2908,27 @@
       <c r="C57" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D57" s="6" t="s">
+      <c r="D57" s="16">
+        <v>46048</v>
+      </c>
+      <c r="E57" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="E57" s="4">
+      <c r="F57" s="4">
         <v>9</v>
       </c>
-      <c r="F57" s="4">
+      <c r="G57" s="4">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="H57" s="4">
         <v>15757278066</v>
       </c>
-      <c r="G57" s="2" t="s">
+      <c r="I57" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A58" s="3" t="s">
         <v>197</v>
       </c>
@@ -2518,20 +2938,27 @@
       <c r="C58" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D58" s="6" t="s">
+      <c r="D58" s="16">
+        <v>46048</v>
+      </c>
+      <c r="E58" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="E58" s="4">
+      <c r="F58" s="4">
         <v>9</v>
       </c>
-      <c r="F58" s="4">
+      <c r="G58" s="4">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="H58" s="4">
         <v>13616296429</v>
       </c>
-      <c r="G58" s="4" t="s">
+      <c r="I58" s="4" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A59" s="3" t="s">
         <v>198</v>
       </c>
@@ -2541,20 +2968,27 @@
       <c r="C59" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D59" s="6" t="s">
+      <c r="D59" s="16">
+        <v>46048</v>
+      </c>
+      <c r="E59" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="E59" s="4">
+      <c r="F59" s="4">
         <v>9</v>
       </c>
-      <c r="F59" s="4">
+      <c r="G59" s="4">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="H59" s="4">
         <v>17757227637</v>
       </c>
-      <c r="G59" s="4" t="s">
+      <c r="I59" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A60" s="3" t="s">
         <v>201</v>
       </c>
@@ -2564,20 +2998,27 @@
       <c r="C60" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D60" s="6" t="s">
+      <c r="D60" s="16">
+        <v>46048</v>
+      </c>
+      <c r="E60" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="E60" s="4">
+      <c r="F60" s="4">
         <v>9</v>
       </c>
-      <c r="F60" s="4" t="s">
+      <c r="G60" s="4">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="H60" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="G60" s="4" t="s">
+      <c r="I60" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A61" s="3" t="s">
         <v>202</v>
       </c>
@@ -2587,20 +3028,27 @@
       <c r="C61" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D61" s="6" t="s">
+      <c r="D61" s="16">
+        <v>46048</v>
+      </c>
+      <c r="E61" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="E61" s="4">
+      <c r="F61" s="4">
         <v>9</v>
       </c>
-      <c r="F61" s="4">
+      <c r="G61" s="4">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="H61" s="4">
         <v>17757227637</v>
       </c>
-      <c r="G61" s="2" t="s">
+      <c r="I61" s="2" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A62" s="3" t="s">
         <v>203</v>
       </c>
@@ -2610,20 +3058,27 @@
       <c r="C62" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D62" s="6" t="s">
+      <c r="D62" s="16">
+        <v>46048</v>
+      </c>
+      <c r="E62" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="E62" s="4">
+      <c r="F62" s="4">
         <v>9</v>
       </c>
-      <c r="F62" s="4">
+      <c r="G62" s="4">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="H62" s="4">
         <v>15967207558</v>
       </c>
-      <c r="G62" s="2" t="s">
+      <c r="I62" s="2" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A63" s="3" t="s">
         <v>207</v>
       </c>
@@ -2633,20 +3088,27 @@
       <c r="C63" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D63" s="6" t="s">
+      <c r="D63" s="16">
+        <v>46048</v>
+      </c>
+      <c r="E63" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="E63" s="4">
+      <c r="F63" s="4">
         <v>6.5</v>
       </c>
-      <c r="F63" s="4">
+      <c r="G63" s="4">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="H63" s="4">
         <v>15295258368</v>
       </c>
-      <c r="G63" s="4" t="s">
+      <c r="I63" s="4" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.4">
       <c r="A64" s="3" t="s">
         <v>211</v>
       </c>
@@ -2656,16 +3118,23 @@
       <c r="C64" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D64" s="3" t="s">
+      <c r="D64" s="16">
+        <v>46048</v>
+      </c>
+      <c r="E64" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="E64" s="4">
+      <c r="F64" s="4">
         <v>23</v>
       </c>
-      <c r="F64" s="4">
+      <c r="G64" s="4">
+        <f t="shared" si="0"/>
+        <v>92</v>
+      </c>
+      <c r="H64" s="4">
         <v>18268360779</v>
       </c>
-      <c r="G64" s="2" t="s">
+      <c r="I64" s="2" t="s">
         <v>212</v>
       </c>
     </row>

</xml_diff>